<commit_message>
solved more tree problems. graph problem of rooms and keys still incomplete
</commit_message>
<xml_diff>
--- a/Problem Solving Approaches.xlsx
+++ b/Problem Solving Approaches.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zaidhumayun/Desktop/Development.nosync/Python/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568B9B3B-16B6-8647-B016-2EFBB5B6655C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE9A68C-EFDD-6B47-93A2-698AD9780821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="29140" windowHeight="17440" xr2:uid="{BBA3A7B1-4C9F-7945-B58D-42304D426978}"/>
+    <workbookView xWindow="1100" yWindow="760" windowWidth="29140" windowHeight="17280" xr2:uid="{BBA3A7B1-4C9F-7945-B58D-42304D426978}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
   <si>
     <t>Problem</t>
   </si>
@@ -233,6 +233,24 @@
   </si>
   <si>
     <t>Inorder Successor in BST</t>
+  </si>
+  <si>
+    <t>Longest Univalue Path In Tree</t>
+  </si>
+  <si>
+    <t>Longest Univalue Path</t>
+  </si>
+  <si>
+    <t>When counting edges, at each point remember to calculate the maximum answer by doing left_path + right_path but when returning an answer to a parent node, return the max(left_path, right_path)</t>
+  </si>
+  <si>
+    <t>Binary Tree Maximum Path Sum</t>
+  </si>
+  <si>
+    <t>Follow logic of longest univalue path or diameter of binary tree. At each node, find the maximum including left and right paths but when returning, return only one of those</t>
+  </si>
+  <si>
+    <t>For problems like this, remember that the local answer and the answer you return to the parent are two separate things</t>
   </si>
 </sst>
 </file>
@@ -316,7 +334,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -363,6 +381,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -684,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6D882F9-E12B-244F-B6D7-64A170453E03}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -778,7 +802,7 @@
       <c r="B8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="24" t="s">
         <v>56</v>
       </c>
       <c r="D8" s="14" t="s">
@@ -801,7 +825,7 @@
       <c r="B9" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="24" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="14" t="s">
@@ -980,12 +1004,45 @@
         <v>61</v>
       </c>
     </row>
+    <row r="22" spans="1:5" ht="66" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="66" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="23"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="G8:I10"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="A15:E15"/>
+    <mergeCell ref="E22:E23"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{449AF18F-A2F3-F14A-B528-643E7615EDD9}"/>
@@ -1005,6 +1062,8 @@
     <hyperlink ref="D19" r:id="rId15" xr:uid="{DDE6CC17-4F8F-B441-810E-748CA26F26B5}"/>
     <hyperlink ref="D20" r:id="rId16" xr:uid="{6ABCAC3A-D7D9-7945-8B06-4B34517BECAA}"/>
     <hyperlink ref="D21" r:id="rId17" xr:uid="{92A2F511-169A-7C41-ABD1-015DF646BD5A}"/>
+    <hyperlink ref="D22" r:id="rId18" xr:uid="{7B14AAAC-BB09-0A42-91E6-269302FC7135}"/>
+    <hyperlink ref="D23" r:id="rId19" xr:uid="{03E7B930-4785-B94D-B55E-079A11D260B5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more graph and dp solutions
</commit_message>
<xml_diff>
--- a/Problem Solving Approaches.xlsx
+++ b/Problem Solving Approaches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zaidhumayun/Desktop/Development.nosync/Python/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F079BEE6-F8B7-854B-B0A1-2EABF85304A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3B8332-31AA-054B-B7DF-5453B3AC2DD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="760" windowWidth="29140" windowHeight="17280" xr2:uid="{BBA3A7B1-4C9F-7945-B58D-42304D426978}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="80">
   <si>
     <t>Problem</t>
   </si>
@@ -277,6 +277,18 @@
   <si>
     <t>Here, since there are two players, they both need to make optimal choices. Also, any choice one player makes minimises the result for the other player because it’s a 2-player zero-sum game.
 Make a nax choice for yourself and pick a choice for your opponent that will minimise the result for you</t>
+  </si>
+  <si>
+    <t>Number Of Ways To Make Change Without Repeating</t>
+  </si>
+  <si>
+    <t>Think of the backtracking approach where you use (index, amount) as the parameters to a function. Make a binary choice at each index to either use the coin or not. Replace for loop with index parameter.</t>
+  </si>
+  <si>
+    <t>Number Of Ways To Make Change</t>
+  </si>
+  <si>
+    <t>Don't use for loop. Use (index, amount) as state variables like the backtracking approach</t>
   </si>
 </sst>
 </file>
@@ -360,7 +372,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -422,6 +434,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -743,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6D882F9-E12B-244F-B6D7-64A170453E03}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -921,7 +936,7 @@
       <c r="A13" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="28" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -1117,6 +1132,23 @@
       </c>
       <c r="E27" s="7" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="88" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1151,6 +1183,7 @@
     <hyperlink ref="D26" r:id="rId20" xr:uid="{1B54A9ED-79DD-0840-BF51-41EE0AB1A347}"/>
     <hyperlink ref="D27" r:id="rId21" xr:uid="{DB350800-AE0F-114F-AE55-F8AE0E8846D6}"/>
     <hyperlink ref="E27" r:id="rId22" display="https://www.geeksforgeeks.org/optimal-strategy-for-a-game-dp-31/" xr:uid="{0C893359-780A-DB4B-8A95-ADB80886AB16}"/>
+    <hyperlink ref="D28" r:id="rId23" xr:uid="{80BE9D2A-AE69-F94A-9129-F50D3D679763}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>